<commit_message>
Alteracoes em parametros na verificacao da tensao no teste de duty cycle, refresh d resultado dos testes
</commit_message>
<xml_diff>
--- a/log/resultados_testes.xlsx
+++ b/log/resultados_testes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB62"/>
+  <dimension ref="A1:AB78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7765,10 +7765,8 @@
           <t>2025-09-08 15:07:23</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>1000000</t>
-        </is>
+      <c r="B62" t="n">
+        <v>1000000</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -7884,6 +7882,2008 @@
         </is>
       </c>
       <c r="AB62" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-09-16 10:25:24</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O63" t="n">
+        <v>20.40150390625</v>
+      </c>
+      <c r="P63" t="n">
+        <v>62.9570000000001</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>23.29661754261364</v>
+      </c>
+      <c r="R63" t="n">
+        <v>69.79999999999997</v>
+      </c>
+      <c r="S63" t="n">
+        <v>22.69723854758523</v>
+      </c>
+      <c r="T63" t="n">
+        <v>67.79999999999994</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z63" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB63" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-09-16 11:08:24</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O64" t="n">
+        <v>20.44674005681818</v>
+      </c>
+      <c r="P64" t="n">
+        <v>62.96400000000008</v>
+      </c>
+      <c r="Q64" t="n">
+        <v>24.04301402698864</v>
+      </c>
+      <c r="R64" t="n">
+        <v>72</v>
+      </c>
+      <c r="S64" t="n">
+        <v>22.79901988636363</v>
+      </c>
+      <c r="T64" t="n">
+        <v>67.99999999999994</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z64" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB64" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-09-16 11:16:11</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O65" t="n">
+        <v>19.70034357244318</v>
+      </c>
+      <c r="P65" t="n">
+        <v>62.97600000000006</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>23.20614524147727</v>
+      </c>
+      <c r="R65" t="n">
+        <v>69.59999999999997</v>
+      </c>
+      <c r="S65" t="n">
+        <v>22.79901988636363</v>
+      </c>
+      <c r="T65" t="n">
+        <v>67.99999999999994</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y65" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z65" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA65" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB65" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-09-16 11:27:35</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O66" t="n">
+        <v>24.52930264559659</v>
+      </c>
+      <c r="P66" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>24.06563210227273</v>
+      </c>
+      <c r="R66" t="n">
+        <v>72</v>
+      </c>
+      <c r="S66" t="n">
+        <v>22.71985662286932</v>
+      </c>
+      <c r="T66" t="n">
+        <v>67.79999999999994</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y66" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z66" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA66" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB66" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-09-16 11:29:43</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O67" t="n">
+        <v>19.88128817471591</v>
+      </c>
+      <c r="P67" t="n">
+        <v>62.95300000000011</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>23.33054465553978</v>
+      </c>
+      <c r="R67" t="n">
+        <v>69.79999999999997</v>
+      </c>
+      <c r="S67" t="n">
+        <v>22.70854758522727</v>
+      </c>
+      <c r="T67" t="n">
+        <v>67.79999999999994</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z67" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA67" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB67" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-09-16 11:32:28</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Thiago</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O68" t="n">
+        <v>20.53721235795454</v>
+      </c>
+      <c r="P68" t="n">
+        <v>62.94900000000012</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>23.18352716619318</v>
+      </c>
+      <c r="R68" t="n">
+        <v>69.59999999999997</v>
+      </c>
+      <c r="S68" t="n">
+        <v>22.71985662286932</v>
+      </c>
+      <c r="T68" t="n">
+        <v>67.79999999999994</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z68" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA68" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB68" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-09-16 12:36:47</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Thiago</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O69" t="n">
+        <v>20.31103160511363</v>
+      </c>
+      <c r="P69" t="n">
+        <v>62.96800000000007</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>24.06563210227273</v>
+      </c>
+      <c r="R69" t="n">
+        <v>72</v>
+      </c>
+      <c r="S69" t="n">
+        <v>22.70854758522727</v>
+      </c>
+      <c r="T69" t="n">
+        <v>67.79999999999994</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z69" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA69" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB69" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-09-16 12:46:41</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O70" t="n">
+        <v>20.58244850852273</v>
+      </c>
+      <c r="P70" t="n">
+        <v>62.96000000000009</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>23.35316273082386</v>
+      </c>
+      <c r="R70" t="n">
+        <v>69.99999999999997</v>
+      </c>
+      <c r="S70" t="n">
+        <v>22.79901988636363</v>
+      </c>
+      <c r="T70" t="n">
+        <v>67.99999999999994</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z70" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA70" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB70" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-09-16 12:48:14</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O71" t="n">
+        <v>24.60846590909091</v>
+      </c>
+      <c r="P71" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>24.133486328125</v>
+      </c>
+      <c r="R71" t="n">
+        <v>72</v>
+      </c>
+      <c r="S71" t="n">
+        <v>24.133486328125</v>
+      </c>
+      <c r="T71" t="n">
+        <v>72</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y71" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z71" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA71" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB71" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-09-16 12:49:35</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="O72" t="n">
+        <v>24.60846590909091</v>
+      </c>
+      <c r="P72" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>24.133486328125</v>
+      </c>
+      <c r="R72" t="n">
+        <v>72</v>
+      </c>
+      <c r="S72" t="n">
+        <v>24.133486328125</v>
+      </c>
+      <c r="T72" t="n">
+        <v>72</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y72" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z72" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA72" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB72" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:04:09</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="O73" t="n">
+        <v>24.61977494673295</v>
+      </c>
+      <c r="P73" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>24.12217729048295</v>
+      </c>
+      <c r="R73" t="n">
+        <v>72</v>
+      </c>
+      <c r="S73" t="n">
+        <v>24.12217729048295</v>
+      </c>
+      <c r="T73" t="n">
+        <v>72</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z73" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA73" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB73" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:16:16</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="O74" t="n">
+        <v>24.61977494673295</v>
+      </c>
+      <c r="P74" t="n">
+        <v>63</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>24.133486328125</v>
+      </c>
+      <c r="R74" t="n">
+        <v>72</v>
+      </c>
+      <c r="S74" t="n">
+        <v>24.133486328125</v>
+      </c>
+      <c r="T74" t="n">
+        <v>72</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>NG</t>
+        </is>
+      </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y74" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z74" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA74" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB74" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:17:52</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr"/>
+      <c r="R75" t="inlineStr"/>
+      <c r="S75" t="inlineStr"/>
+      <c r="T75" t="inlineStr"/>
+      <c r="U75" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB75" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:17:58</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
+      <c r="R76" t="inlineStr"/>
+      <c r="S76" t="inlineStr"/>
+      <c r="T76" t="inlineStr"/>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB76" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:18:07</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>325100100673</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr"/>
+      <c r="R77" t="inlineStr"/>
+      <c r="S77" t="inlineStr"/>
+      <c r="T77" t="inlineStr"/>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB77" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-09-16 13:18:23</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>0325100100676</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Thiago Dias</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr"/>
+      <c r="R78" t="inlineStr"/>
+      <c r="S78" t="inlineStr"/>
+      <c r="T78" t="inlineStr"/>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="W78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Y78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="Z78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AA78" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="AB78" t="inlineStr">
         <is>
           <t>PENDING</t>
         </is>

</xml_diff>